<commit_message>
Working on Doku, deleting bidets, trying resnet
</commit_message>
<xml_diff>
--- a/Statistik/AnsaetzeNormalisierungDatenmengeProKategorie.xlsx
+++ b/Statistik/AnsaetzeNormalisierungDatenmengeProKategorie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\anni\Documents\GitHub\CoopDFKI\Statistik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22956738-8D40-4E82-9528-F967C3CD17E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA47DA80-7963-4F12-94B3-582D79BAB084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="12735" xr2:uid="{DEAAA407-0FA1-4C6F-9EEE-322A39F6D044}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DEAAA407-0FA1-4C6F-9EEE-322A39F6D044}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Normalisierung der Trainingsdatenmengen</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>Ansatz Skalierung über Mittelwert mit Normalbereich von 73 bis 193</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Vervielfältigung</t>
   </si>
 </sst>
 </file>
@@ -107,6 +116,1995 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Vervielfältigungsfaktoren</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$34:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>162.22222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.739130434782609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.174603174603174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.791044776119403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.138364779874214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.131233595800525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0FD-4265-B661-51B8A851C3ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1250037711"/>
+        <c:axId val="1169949087"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1250037711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1169949087"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1169949087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250037711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vervielfältigung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$33:$M$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>381</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$34:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>162.22222222222223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.739130434782609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.174603174603174</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.791044776119403</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.138364779874214</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.131233595800525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9EC4-4A14-B826-2480FC94568A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1281486271"/>
+        <c:axId val="1071892735"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1281486271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" baseline="0"/>
+                  <a:t> der Bilder in den Katgorien</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1071892735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1071892735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Berechneter Vervielfältigungsfaktor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1281486271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88CE6A48-9C84-41F4-8D4A-1B4E8EEFFE09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B832E6-478A-407D-BFEF-C2E219D942AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC43CD5-107C-43CA-9127-0BF71F1257A5}">
   <dimension ref="A2:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +2665,7 @@
         <v>41.811023622047244</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <f>B15*B16</f>
         <v>5656.8241469816276</v>
@@ -717,18 +2715,18 @@
         <v>3261.2598425196852</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>SUM(B18:M18)</f>
         <v>42727.139107611547</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>185</v>
       </c>
@@ -766,7 +2764,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f>20*133/B24</f>
         <v>14.378378378378379</v>
@@ -816,7 +2814,7 @@
         <v>34.102564102564102</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>B25*B24</f>
         <v>2660</v>
@@ -866,88 +2864,131 @@
         <v>2660</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29">
         <f>SUM(B27:M27)</f>
         <v>31920</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>12</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>7</v>
+      </c>
+    </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
       <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>46</v>
+      </c>
+      <c r="D33">
+        <v>63</v>
+      </c>
+      <c r="E33">
+        <v>67</v>
+      </c>
+      <c r="F33">
+        <v>70</v>
+      </c>
+      <c r="G33">
+        <v>77</v>
+      </c>
+      <c r="H33">
+        <v>78</v>
+      </c>
+      <c r="I33">
+        <v>145</v>
+      </c>
+      <c r="J33">
+        <v>161</v>
+      </c>
+      <c r="K33">
         <v>185</v>
       </c>
-      <c r="C33">
-        <v>67</v>
-      </c>
-      <c r="D33">
-        <v>70</v>
-      </c>
-      <c r="E33">
+      <c r="L33">
         <v>318</v>
       </c>
-      <c r="F33">
-        <v>9</v>
-      </c>
-      <c r="G33">
-        <v>161</v>
-      </c>
-      <c r="H33">
+      <c r="M33">
         <v>381</v>
-      </c>
-      <c r="I33">
-        <v>46</v>
-      </c>
-      <c r="J33">
-        <v>77</v>
-      </c>
-      <c r="K33">
-        <v>145</v>
-      </c>
-      <c r="L33">
-        <v>63</v>
-      </c>
-      <c r="M33">
-        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>50</v>
+      <c r="A34" t="s">
+        <v>9</v>
       </c>
       <c r="B34" s="1">
-        <v>20</v>
+        <f>20*73/B33</f>
+        <v>162.22222222222223</v>
       </c>
       <c r="C34" s="1">
         <f>20*73/C33</f>
-        <v>21.791044776119403</v>
+        <v>31.739130434782609</v>
       </c>
       <c r="D34" s="1">
         <f>20*73/D33</f>
-        <v>20.857142857142858</v>
+        <v>23.174603174603174</v>
       </c>
       <c r="E34" s="1">
-        <f>20*193/E33</f>
-        <v>12.138364779874214</v>
+        <f>20*73/E33</f>
+        <v>21.791044776119403</v>
       </c>
       <c r="F34" s="1">
         <f>20*73/F33</f>
-        <v>162.22222222222223</v>
+        <v>20.857142857142858</v>
       </c>
       <c r="G34" s="1">
         <v>20</v>
       </c>
       <c r="H34" s="1">
-        <f>20*193/H33</f>
-        <v>10.131233595800525</v>
+        <v>20</v>
       </c>
       <c r="I34" s="1">
-        <f>20*73/I33</f>
-        <v>31.739130434782609</v>
+        <v>20</v>
       </c>
       <c r="J34" s="1">
         <v>20</v>
@@ -956,61 +2997,62 @@
         <v>20</v>
       </c>
       <c r="L34" s="1">
-        <f>20*73/L33</f>
-        <v>23.174603174603174</v>
+        <f>20*193/L33</f>
+        <v>12.138364779874214</v>
       </c>
       <c r="M34" s="1">
-        <v>20</v>
+        <f>20*193/M33</f>
+        <v>10.131233595800525</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B36">
         <f>B34*B33</f>
-        <v>3700</v>
+        <v>1460</v>
       </c>
       <c r="C36">
         <f>C34*C33</f>
         <v>1460</v>
       </c>
       <c r="D36">
-        <f t="shared" ref="D36:M36" si="6">D34*D33</f>
+        <f>D34*D33</f>
         <v>1460</v>
       </c>
       <c r="E36">
-        <f t="shared" si="6"/>
+        <f>E34*E33</f>
+        <v>1460</v>
+      </c>
+      <c r="F36">
+        <f>F34*F33</f>
+        <v>1460</v>
+      </c>
+      <c r="G36">
+        <f>G34*G33</f>
+        <v>1540</v>
+      </c>
+      <c r="H36">
+        <f>H34*H33</f>
+        <v>1560</v>
+      </c>
+      <c r="I36">
+        <f>I34*I33</f>
+        <v>2900</v>
+      </c>
+      <c r="J36">
+        <f>J34*J33</f>
+        <v>3220</v>
+      </c>
+      <c r="K36">
+        <f>K34*K33</f>
+        <v>3700</v>
+      </c>
+      <c r="L36">
+        <f>L34*L33</f>
         <v>3860</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="6"/>
-        <v>1460</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="6"/>
-        <v>3220</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="6"/>
+      <c r="M36">
+        <f>M34*M33</f>
         <v>3860</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="6"/>
-        <v>1460</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="6"/>
-        <v>1540</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="6"/>
-        <v>2900</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="6"/>
-        <v>1460</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="6"/>
-        <v>1560</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1020,7 +3062,11 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B32:M34">
+    <sortCondition ref="B33:M33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>